<commit_message>
650903:0550 Start to Fix Contract Document
</commit_message>
<xml_diff>
--- a/templates/documents/af_report.xlsx
+++ b/templates/documents/af_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWeb\BK_Housing\templates\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302C1182-3514-413F-9682-2FACF80D0EAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93D079E-4EC0-4C06-8F0A-1A5CB7EAD8D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4440" windowWidth="19440" windowHeight="15000" xr2:uid="{4F5E3766-BB80-4266-BB77-76F27709B2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F5E3766-BB80-4266-BB77-76F27709B2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10773" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10988" uniqueCount="81">
   <si>
     <t>กลุ่มชั้นยศ</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>XXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXXX</t>
+  </si>
+  <si>
+    <t>armis modify</t>
   </si>
 </sst>
 </file>
@@ -758,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE69CFE9-DA39-4534-BBBF-2AACAB9724E0}">
-  <dimension ref="A1:AX1205"/>
+  <dimension ref="A1:AY1205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,9 +819,10 @@
     <col min="48" max="48" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:51" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -969,8 +973,11 @@
       <c r="AX1" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY1" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A2" s="14" t="s">
         <v>48</v>
       </c>
@@ -1055,7 +1062,7 @@
       </c>
       <c r="AL2" s="14"/>
     </row>
-    <row r="3" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A3" s="14" t="s">
         <v>71</v>
       </c>
@@ -1206,8 +1213,11 @@
       <c r="AX3" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY3" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A4" s="14" t="s">
         <v>71</v>
       </c>
@@ -1358,8 +1368,11 @@
       <c r="AX4" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY4" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A5" s="14" t="s">
         <v>71</v>
       </c>
@@ -1510,8 +1523,11 @@
       <c r="AX5" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY5" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A6" s="14" t="s">
         <v>71</v>
       </c>
@@ -1662,8 +1678,11 @@
       <c r="AX6" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY6" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
@@ -1814,8 +1833,11 @@
       <c r="AX7" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY7" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A8" s="14" t="s">
         <v>71</v>
       </c>
@@ -1966,8 +1988,11 @@
       <c r="AX8" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY8" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A9" s="14" t="s">
         <v>71</v>
       </c>
@@ -2118,8 +2143,11 @@
       <c r="AX9" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY9" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A10" s="14" t="s">
         <v>71</v>
       </c>
@@ -2270,8 +2298,11 @@
       <c r="AX10" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY10" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A11" s="14" t="s">
         <v>71</v>
       </c>
@@ -2422,8 +2453,11 @@
       <c r="AX11" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY11" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A12" s="14" t="s">
         <v>71</v>
       </c>
@@ -2574,8 +2608,11 @@
       <c r="AX12" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY12" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A13" s="14" t="s">
         <v>71</v>
       </c>
@@ -2726,8 +2763,11 @@
       <c r="AX13" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY13" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A14" s="14" t="s">
         <v>71</v>
       </c>
@@ -2878,8 +2918,11 @@
       <c r="AX14" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY14" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A15" s="14" t="s">
         <v>71</v>
       </c>
@@ -3030,8 +3073,11 @@
       <c r="AX15" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY15" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A16" s="14" t="s">
         <v>71</v>
       </c>
@@ -3182,8 +3228,11 @@
       <c r="AX16" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY16" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A17" s="14" t="s">
         <v>71</v>
       </c>
@@ -3334,8 +3383,11 @@
       <c r="AX17" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY17" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A18" s="14" t="s">
         <v>71</v>
       </c>
@@ -3486,8 +3538,11 @@
       <c r="AX18" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY18" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A19" s="14" t="s">
         <v>71</v>
       </c>
@@ -3638,8 +3693,11 @@
       <c r="AX19" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY19" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A20" s="14" t="s">
         <v>71</v>
       </c>
@@ -3790,8 +3848,11 @@
       <c r="AX20" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY20" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A21" s="14" t="s">
         <v>71</v>
       </c>
@@ -3942,8 +4003,11 @@
       <c r="AX21" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY21" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A22" s="14" t="s">
         <v>71</v>
       </c>
@@ -4094,8 +4158,11 @@
       <c r="AX22" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY22" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A23" s="14" t="s">
         <v>71</v>
       </c>
@@ -4246,8 +4313,11 @@
       <c r="AX23" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY23" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A24" s="14" t="s">
         <v>71</v>
       </c>
@@ -4398,8 +4468,11 @@
       <c r="AX24" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY24" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A25" s="14" t="s">
         <v>71</v>
       </c>
@@ -4550,8 +4623,11 @@
       <c r="AX25" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY25" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A26" s="14" t="s">
         <v>71</v>
       </c>
@@ -4702,8 +4778,11 @@
       <c r="AX26" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY26" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A27" s="14" t="s">
         <v>71</v>
       </c>
@@ -4854,8 +4933,11 @@
       <c r="AX27" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY27" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A28" s="14" t="s">
         <v>71</v>
       </c>
@@ -5006,8 +5088,11 @@
       <c r="AX28" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY28" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A29" s="14" t="s">
         <v>71</v>
       </c>
@@ -5158,8 +5243,11 @@
       <c r="AX29" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY29" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A30" s="14" t="s">
         <v>71</v>
       </c>
@@ -5310,8 +5398,11 @@
       <c r="AX30" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY30" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A31" s="14" t="s">
         <v>71</v>
       </c>
@@ -5462,8 +5553,11 @@
       <c r="AX31" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY31" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A32" s="14" t="s">
         <v>71</v>
       </c>
@@ -5614,8 +5708,11 @@
       <c r="AX32" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY32" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A33" s="14" t="s">
         <v>71</v>
       </c>
@@ -5766,8 +5863,11 @@
       <c r="AX33" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY33" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A34" s="14" t="s">
         <v>71</v>
       </c>
@@ -5918,8 +6018,11 @@
       <c r="AX34" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="35" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY34" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A35" s="14" t="s">
         <v>71</v>
       </c>
@@ -6070,8 +6173,11 @@
       <c r="AX35" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY35" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A36" s="14" t="s">
         <v>71</v>
       </c>
@@ -6222,8 +6328,11 @@
       <c r="AX36" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY36" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A37" s="14" t="s">
         <v>71</v>
       </c>
@@ -6374,8 +6483,11 @@
       <c r="AX37" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="38" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY37" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A38" s="14" t="s">
         <v>71</v>
       </c>
@@ -6526,8 +6638,11 @@
       <c r="AX38" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY38" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A39" s="14" t="s">
         <v>71</v>
       </c>
@@ -6678,8 +6793,11 @@
       <c r="AX39" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY39" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A40" s="14" t="s">
         <v>71</v>
       </c>
@@ -6830,8 +6948,11 @@
       <c r="AX40" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY40" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A41" s="14" t="s">
         <v>71</v>
       </c>
@@ -6982,8 +7103,11 @@
       <c r="AX41" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY41" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A42" s="14" t="s">
         <v>71</v>
       </c>
@@ -7134,8 +7258,11 @@
       <c r="AX42" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="43" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY42" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A43" s="14" t="s">
         <v>71</v>
       </c>
@@ -7286,8 +7413,11 @@
       <c r="AX43" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY43" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A44" s="14" t="s">
         <v>71</v>
       </c>
@@ -7438,8 +7568,11 @@
       <c r="AX44" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="45" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY44" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A45" s="14" t="s">
         <v>71</v>
       </c>
@@ -7590,8 +7723,11 @@
       <c r="AX45" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="46" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY45" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A46" s="14" t="s">
         <v>71</v>
       </c>
@@ -7742,8 +7878,11 @@
       <c r="AX46" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="47" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY46" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A47" s="14" t="s">
         <v>71</v>
       </c>
@@ -7894,8 +8033,11 @@
       <c r="AX47" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY47" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A48" s="14" t="s">
         <v>71</v>
       </c>
@@ -8046,8 +8188,11 @@
       <c r="AX48" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="49" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY48" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A49" s="14" t="s">
         <v>71</v>
       </c>
@@ -8198,8 +8343,11 @@
       <c r="AX49" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY49" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A50" s="14" t="s">
         <v>71</v>
       </c>
@@ -8350,8 +8498,11 @@
       <c r="AX50" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="51" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY50" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A51" s="14" t="s">
         <v>71</v>
       </c>
@@ -8502,8 +8653,11 @@
       <c r="AX51" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="52" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY51" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A52" s="14" t="s">
         <v>71</v>
       </c>
@@ -8654,8 +8808,11 @@
       <c r="AX52" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY52" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A53" s="14" t="s">
         <v>71</v>
       </c>
@@ -8806,8 +8963,11 @@
       <c r="AX53" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="54" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY53" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A54" s="14" t="s">
         <v>71</v>
       </c>
@@ -8958,8 +9118,11 @@
       <c r="AX54" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY54" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A55" s="14" t="s">
         <v>71</v>
       </c>
@@ -9110,8 +9273,11 @@
       <c r="AX55" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY55" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A56" s="14" t="s">
         <v>71</v>
       </c>
@@ -9262,8 +9428,11 @@
       <c r="AX56" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="57" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY56" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A57" s="14" t="s">
         <v>71</v>
       </c>
@@ -9414,8 +9583,11 @@
       <c r="AX57" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="58" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY57" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A58" s="14" t="s">
         <v>71</v>
       </c>
@@ -9566,8 +9738,11 @@
       <c r="AX58" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY58" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A59" s="14" t="s">
         <v>71</v>
       </c>
@@ -9718,8 +9893,11 @@
       <c r="AX59" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="60" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY59" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A60" s="14" t="s">
         <v>71</v>
       </c>
@@ -9870,8 +10048,11 @@
       <c r="AX60" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="61" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY60" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A61" s="14" t="s">
         <v>71</v>
       </c>
@@ -10022,8 +10203,11 @@
       <c r="AX61" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="62" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY61" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A62" s="14" t="s">
         <v>71</v>
       </c>
@@ -10174,8 +10358,11 @@
       <c r="AX62" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="63" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY62" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A63" s="14" t="s">
         <v>71</v>
       </c>
@@ -10326,8 +10513,11 @@
       <c r="AX63" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="64" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY63" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A64" s="14" t="s">
         <v>71</v>
       </c>
@@ -10478,8 +10668,11 @@
       <c r="AX64" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="65" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY64" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A65" s="14" t="s">
         <v>71</v>
       </c>
@@ -10630,8 +10823,11 @@
       <c r="AX65" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="66" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY65" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A66" s="14" t="s">
         <v>71</v>
       </c>
@@ -10782,8 +10978,11 @@
       <c r="AX66" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="67" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY66" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A67" s="14" t="s">
         <v>71</v>
       </c>
@@ -10934,8 +11133,11 @@
       <c r="AX67" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="68" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY67" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A68" s="14" t="s">
         <v>71</v>
       </c>
@@ -11086,8 +11288,11 @@
       <c r="AX68" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="69" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY68" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A69" s="14" t="s">
         <v>71</v>
       </c>
@@ -11238,8 +11443,11 @@
       <c r="AX69" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY69" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A70" s="14" t="s">
         <v>71</v>
       </c>
@@ -11390,8 +11598,11 @@
       <c r="AX70" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="71" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY70" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A71" s="14" t="s">
         <v>71</v>
       </c>
@@ -11542,8 +11753,11 @@
       <c r="AX71" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="72" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY71" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A72" s="14" t="s">
         <v>71</v>
       </c>
@@ -11694,8 +11908,11 @@
       <c r="AX72" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="73" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY72" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A73" s="14" t="s">
         <v>71</v>
       </c>
@@ -11846,8 +12063,11 @@
       <c r="AX73" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="74" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY73" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A74" s="14" t="s">
         <v>71</v>
       </c>
@@ -11998,8 +12218,11 @@
       <c r="AX74" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="75" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY74" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A75" s="14" t="s">
         <v>71</v>
       </c>
@@ -12150,8 +12373,11 @@
       <c r="AX75" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="76" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY75" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A76" s="14" t="s">
         <v>71</v>
       </c>
@@ -12302,8 +12528,11 @@
       <c r="AX76" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="77" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY76" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A77" s="14" t="s">
         <v>71</v>
       </c>
@@ -12454,8 +12683,11 @@
       <c r="AX77" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="78" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY77" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A78" s="14" t="s">
         <v>71</v>
       </c>
@@ -12606,8 +12838,11 @@
       <c r="AX78" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY78" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A79" s="14" t="s">
         <v>71</v>
       </c>
@@ -12758,8 +12993,11 @@
       <c r="AX79" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY79" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A80" s="14" t="s">
         <v>71</v>
       </c>
@@ -12910,8 +13148,11 @@
       <c r="AX80" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY80" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A81" s="14" t="s">
         <v>71</v>
       </c>
@@ -13062,8 +13303,11 @@
       <c r="AX81" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY81" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A82" s="14" t="s">
         <v>71</v>
       </c>
@@ -13214,8 +13458,11 @@
       <c r="AX82" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="83" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY82" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A83" s="14" t="s">
         <v>71</v>
       </c>
@@ -13366,8 +13613,11 @@
       <c r="AX83" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="84" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY83" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A84" s="14" t="s">
         <v>71</v>
       </c>
@@ -13518,8 +13768,11 @@
       <c r="AX84" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="85" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY84" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A85" s="14" t="s">
         <v>71</v>
       </c>
@@ -13670,8 +13923,11 @@
       <c r="AX85" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="86" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY85" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="86" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A86" s="14" t="s">
         <v>71</v>
       </c>
@@ -13822,8 +14078,11 @@
       <c r="AX86" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="87" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY86" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A87" s="14" t="s">
         <v>71</v>
       </c>
@@ -13974,8 +14233,11 @@
       <c r="AX87" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="88" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY87" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A88" s="14" t="s">
         <v>71</v>
       </c>
@@ -14126,8 +14388,11 @@
       <c r="AX88" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="89" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY88" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="89" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A89" s="14" t="s">
         <v>71</v>
       </c>
@@ -14278,8 +14543,11 @@
       <c r="AX89" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="90" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY89" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A90" s="14" t="s">
         <v>71</v>
       </c>
@@ -14430,8 +14698,11 @@
       <c r="AX90" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="91" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY90" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A91" s="14" t="s">
         <v>71</v>
       </c>
@@ -14582,8 +14853,11 @@
       <c r="AX91" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="92" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY91" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A92" s="14" t="s">
         <v>71</v>
       </c>
@@ -14734,8 +15008,11 @@
       <c r="AX92" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="93" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY92" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A93" s="14" t="s">
         <v>71</v>
       </c>
@@ -14886,8 +15163,11 @@
       <c r="AX93" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="94" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY93" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A94" s="14" t="s">
         <v>71</v>
       </c>
@@ -15038,8 +15318,11 @@
       <c r="AX94" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="95" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY94" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A95" s="14" t="s">
         <v>71</v>
       </c>
@@ -15190,8 +15473,11 @@
       <c r="AX95" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="96" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY95" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="96" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A96" s="14" t="s">
         <v>71</v>
       </c>
@@ -15342,8 +15628,11 @@
       <c r="AX96" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="97" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY96" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="97" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A97" s="14" t="s">
         <v>71</v>
       </c>
@@ -15494,8 +15783,11 @@
       <c r="AX97" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="98" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY97" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A98" s="14" t="s">
         <v>71</v>
       </c>
@@ -15646,8 +15938,11 @@
       <c r="AX98" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="99" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY98" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="99" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A99" s="14" t="s">
         <v>71</v>
       </c>
@@ -15798,8 +16093,11 @@
       <c r="AX99" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="100" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY99" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="100" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A100" s="14" t="s">
         <v>71</v>
       </c>
@@ -15950,8 +16248,11 @@
       <c r="AX100" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="101" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY100" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="101" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A101" s="14" t="s">
         <v>71</v>
       </c>
@@ -16102,8 +16403,11 @@
       <c r="AX101" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="102" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY101" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A102" s="14" t="s">
         <v>71</v>
       </c>
@@ -16254,8 +16558,11 @@
       <c r="AX102" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="103" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY102" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="103" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A103" s="14" t="s">
         <v>71</v>
       </c>
@@ -16406,8 +16713,11 @@
       <c r="AX103" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="104" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY103" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="104" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A104" s="14" t="s">
         <v>71</v>
       </c>
@@ -16558,8 +16868,11 @@
       <c r="AX104" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="105" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY104" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="105" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A105" s="14" t="s">
         <v>71</v>
       </c>
@@ -16710,8 +17023,11 @@
       <c r="AX105" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="106" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY105" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="106" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A106" s="14" t="s">
         <v>71</v>
       </c>
@@ -16862,8 +17178,11 @@
       <c r="AX106" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="107" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY106" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="107" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A107" s="14" t="s">
         <v>71</v>
       </c>
@@ -17014,8 +17333,11 @@
       <c r="AX107" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="108" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY107" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="108" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A108" s="14" t="s">
         <v>71</v>
       </c>
@@ -17166,8 +17488,11 @@
       <c r="AX108" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="109" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY108" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="109" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A109" s="14" t="s">
         <v>71</v>
       </c>
@@ -17318,8 +17643,11 @@
       <c r="AX109" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="110" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY109" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="110" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A110" s="14" t="s">
         <v>71</v>
       </c>
@@ -17470,8 +17798,11 @@
       <c r="AX110" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="111" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY110" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="111" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A111" s="14" t="s">
         <v>71</v>
       </c>
@@ -17622,8 +17953,11 @@
       <c r="AX111" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="112" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY111" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="112" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A112" s="14" t="s">
         <v>71</v>
       </c>
@@ -17774,8 +18108,11 @@
       <c r="AX112" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="113" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY112" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="113" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A113" s="14" t="s">
         <v>71</v>
       </c>
@@ -17926,8 +18263,11 @@
       <c r="AX113" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="114" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY113" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="114" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A114" s="14" t="s">
         <v>71</v>
       </c>
@@ -18078,8 +18418,11 @@
       <c r="AX114" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="115" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY114" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="115" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A115" s="14" t="s">
         <v>71</v>
       </c>
@@ -18230,8 +18573,11 @@
       <c r="AX115" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="116" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY115" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="116" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A116" s="14" t="s">
         <v>71</v>
       </c>
@@ -18382,8 +18728,11 @@
       <c r="AX116" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="117" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY116" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="117" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A117" s="14" t="s">
         <v>71</v>
       </c>
@@ -18534,8 +18883,11 @@
       <c r="AX117" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="118" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY117" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="118" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A118" s="14" t="s">
         <v>71</v>
       </c>
@@ -18686,8 +19038,11 @@
       <c r="AX118" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="119" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY118" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="119" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A119" s="14" t="s">
         <v>71</v>
       </c>
@@ -18838,8 +19193,11 @@
       <c r="AX119" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="120" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY119" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="120" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A120" s="14" t="s">
         <v>71</v>
       </c>
@@ -18990,8 +19348,11 @@
       <c r="AX120" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="121" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY120" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="121" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A121" s="14" t="s">
         <v>71</v>
       </c>
@@ -19142,8 +19503,11 @@
       <c r="AX121" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="122" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY121" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="122" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A122" s="14" t="s">
         <v>71</v>
       </c>
@@ -19294,8 +19658,11 @@
       <c r="AX122" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="123" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY122" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="123" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A123" s="14" t="s">
         <v>71</v>
       </c>
@@ -19446,8 +19813,11 @@
       <c r="AX123" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="124" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY123" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="124" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A124" s="14" t="s">
         <v>71</v>
       </c>
@@ -19598,8 +19968,11 @@
       <c r="AX124" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="125" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY124" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="125" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A125" s="14" t="s">
         <v>71</v>
       </c>
@@ -19750,8 +20123,11 @@
       <c r="AX125" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="126" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY125" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="126" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A126" s="14" t="s">
         <v>71</v>
       </c>
@@ -19902,8 +20278,11 @@
       <c r="AX126" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="127" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY126" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="127" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A127" s="14" t="s">
         <v>71</v>
       </c>
@@ -20054,8 +20433,11 @@
       <c r="AX127" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="128" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY127" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="128" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A128" s="14" t="s">
         <v>71</v>
       </c>
@@ -20206,8 +20588,11 @@
       <c r="AX128" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="129" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY128" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="129" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A129" s="14" t="s">
         <v>71</v>
       </c>
@@ -20358,8 +20743,11 @@
       <c r="AX129" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="130" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY129" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="130" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A130" s="14" t="s">
         <v>71</v>
       </c>
@@ -20510,8 +20898,11 @@
       <c r="AX130" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="131" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY130" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="131" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A131" s="14" t="s">
         <v>71</v>
       </c>
@@ -20662,8 +21053,11 @@
       <c r="AX131" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="132" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY131" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="132" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A132" s="14" t="s">
         <v>71</v>
       </c>
@@ -20814,8 +21208,11 @@
       <c r="AX132" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="133" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY132" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="133" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A133" s="14" t="s">
         <v>71</v>
       </c>
@@ -20966,8 +21363,11 @@
       <c r="AX133" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="134" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY133" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="134" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A134" s="14" t="s">
         <v>71</v>
       </c>
@@ -21118,8 +21518,11 @@
       <c r="AX134" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="135" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY134" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="135" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A135" s="14" t="s">
         <v>71</v>
       </c>
@@ -21270,8 +21673,11 @@
       <c r="AX135" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="136" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY135" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="136" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A136" s="14" t="s">
         <v>71</v>
       </c>
@@ -21422,8 +21828,11 @@
       <c r="AX136" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="137" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY136" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="137" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A137" s="14" t="s">
         <v>71</v>
       </c>
@@ -21574,8 +21983,11 @@
       <c r="AX137" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="138" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY137" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="138" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A138" s="14" t="s">
         <v>71</v>
       </c>
@@ -21726,8 +22138,11 @@
       <c r="AX138" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="139" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY138" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="139" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A139" s="14" t="s">
         <v>71</v>
       </c>
@@ -21878,8 +22293,11 @@
       <c r="AX139" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="140" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY139" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="140" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A140" s="14" t="s">
         <v>71</v>
       </c>
@@ -22030,8 +22448,11 @@
       <c r="AX140" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="141" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY140" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="141" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A141" s="14" t="s">
         <v>71</v>
       </c>
@@ -22182,8 +22603,11 @@
       <c r="AX141" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="142" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY141" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="142" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A142" s="14" t="s">
         <v>71</v>
       </c>
@@ -22334,8 +22758,11 @@
       <c r="AX142" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="143" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY142" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="143" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A143" s="14" t="s">
         <v>71</v>
       </c>
@@ -22486,8 +22913,11 @@
       <c r="AX143" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="144" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY143" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="144" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A144" s="14" t="s">
         <v>71</v>
       </c>
@@ -22638,8 +23068,11 @@
       <c r="AX144" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="145" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY144" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="145" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A145" s="14" t="s">
         <v>71</v>
       </c>
@@ -22790,8 +23223,11 @@
       <c r="AX145" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="146" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY145" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="146" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A146" s="14" t="s">
         <v>71</v>
       </c>
@@ -22942,8 +23378,11 @@
       <c r="AX146" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="147" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY146" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="147" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A147" s="14" t="s">
         <v>71</v>
       </c>
@@ -23094,8 +23533,11 @@
       <c r="AX147" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="148" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY147" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="148" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A148" s="14" t="s">
         <v>71</v>
       </c>
@@ -23246,8 +23688,11 @@
       <c r="AX148" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="149" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY148" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="149" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A149" s="14" t="s">
         <v>71</v>
       </c>
@@ -23398,8 +23843,11 @@
       <c r="AX149" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="150" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY149" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="150" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A150" s="14" t="s">
         <v>71</v>
       </c>
@@ -23550,8 +23998,11 @@
       <c r="AX150" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="151" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY150" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="151" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A151" s="14" t="s">
         <v>71</v>
       </c>
@@ -23702,8 +24153,11 @@
       <c r="AX151" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="152" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY151" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="152" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A152" s="14" t="s">
         <v>71</v>
       </c>
@@ -23854,8 +24308,11 @@
       <c r="AX152" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="153" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY152" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="153" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A153" s="14" t="s">
         <v>71</v>
       </c>
@@ -24006,8 +24463,11 @@
       <c r="AX153" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="154" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY153" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="154" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A154" s="14" t="s">
         <v>71</v>
       </c>
@@ -24158,8 +24618,11 @@
       <c r="AX154" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="155" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY154" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="155" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A155" s="14" t="s">
         <v>71</v>
       </c>
@@ -24310,8 +24773,11 @@
       <c r="AX155" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="156" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY155" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="156" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A156" s="14" t="s">
         <v>71</v>
       </c>
@@ -24462,8 +24928,11 @@
       <c r="AX156" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="157" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY156" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="157" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A157" s="14" t="s">
         <v>71</v>
       </c>
@@ -24614,8 +25083,11 @@
       <c r="AX157" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="158" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY157" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="158" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A158" s="14" t="s">
         <v>71</v>
       </c>
@@ -24766,8 +25238,11 @@
       <c r="AX158" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="159" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY158" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="159" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A159" s="14" t="s">
         <v>71</v>
       </c>
@@ -24918,8 +25393,11 @@
       <c r="AX159" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="160" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY159" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="160" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A160" s="14" t="s">
         <v>71</v>
       </c>
@@ -25070,8 +25548,11 @@
       <c r="AX160" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="161" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY160" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="161" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A161" s="14" t="s">
         <v>71</v>
       </c>
@@ -25222,8 +25703,11 @@
       <c r="AX161" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="162" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY161" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="162" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A162" s="14" t="s">
         <v>71</v>
       </c>
@@ -25374,8 +25858,11 @@
       <c r="AX162" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="163" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY162" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="163" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A163" s="14" t="s">
         <v>71</v>
       </c>
@@ -25526,8 +26013,11 @@
       <c r="AX163" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="164" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY163" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="164" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A164" s="14" t="s">
         <v>71</v>
       </c>
@@ -25678,8 +26168,11 @@
       <c r="AX164" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="165" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY164" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="165" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A165" s="14" t="s">
         <v>71</v>
       </c>
@@ -25830,8 +26323,11 @@
       <c r="AX165" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="166" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY165" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="166" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A166" s="14" t="s">
         <v>71</v>
       </c>
@@ -25982,8 +26478,11 @@
       <c r="AX166" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="167" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY166" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="167" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A167" s="14" t="s">
         <v>71</v>
       </c>
@@ -26134,8 +26633,11 @@
       <c r="AX167" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="168" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY167" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="168" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A168" s="14" t="s">
         <v>71</v>
       </c>
@@ -26286,8 +26788,11 @@
       <c r="AX168" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="169" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY168" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="169" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A169" s="14" t="s">
         <v>71</v>
       </c>
@@ -26438,8 +26943,11 @@
       <c r="AX169" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="170" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY169" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="170" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A170" s="14" t="s">
         <v>71</v>
       </c>
@@ -26590,8 +27098,11 @@
       <c r="AX170" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="171" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY170" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="171" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A171" s="14" t="s">
         <v>71</v>
       </c>
@@ -26742,8 +27253,11 @@
       <c r="AX171" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="172" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY171" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="172" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A172" s="14" t="s">
         <v>71</v>
       </c>
@@ -26894,8 +27408,11 @@
       <c r="AX172" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="173" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY172" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="173" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A173" s="14" t="s">
         <v>71</v>
       </c>
@@ -27046,8 +27563,11 @@
       <c r="AX173" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="174" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY173" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="174" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A174" s="14" t="s">
         <v>71</v>
       </c>
@@ -27198,8 +27718,11 @@
       <c r="AX174" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="175" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY174" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="175" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A175" s="14" t="s">
         <v>71</v>
       </c>
@@ -27350,8 +27873,11 @@
       <c r="AX175" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="176" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY175" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="176" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A176" s="14" t="s">
         <v>71</v>
       </c>
@@ -27502,8 +28028,11 @@
       <c r="AX176" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="177" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY176" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="177" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A177" s="14" t="s">
         <v>71</v>
       </c>
@@ -27654,8 +28183,11 @@
       <c r="AX177" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="178" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY177" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="178" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A178" s="14" t="s">
         <v>71</v>
       </c>
@@ -27806,8 +28338,11 @@
       <c r="AX178" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="179" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY178" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="179" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A179" s="14" t="s">
         <v>71</v>
       </c>
@@ -27958,8 +28493,11 @@
       <c r="AX179" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="180" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY179" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="180" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A180" s="14" t="s">
         <v>71</v>
       </c>
@@ -28110,8 +28648,11 @@
       <c r="AX180" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="181" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY180" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="181" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A181" s="14" t="s">
         <v>71</v>
       </c>
@@ -28262,8 +28803,11 @@
       <c r="AX181" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="182" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY181" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="182" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A182" s="14" t="s">
         <v>71</v>
       </c>
@@ -28414,8 +28958,11 @@
       <c r="AX182" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="183" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY182" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="183" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A183" s="14" t="s">
         <v>71</v>
       </c>
@@ -28566,8 +29113,11 @@
       <c r="AX183" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="184" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY183" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="184" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A184" s="14" t="s">
         <v>71</v>
       </c>
@@ -28718,8 +29268,11 @@
       <c r="AX184" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="185" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY184" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="185" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A185" s="14" t="s">
         <v>71</v>
       </c>
@@ -28870,8 +29423,11 @@
       <c r="AX185" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="186" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY185" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="186" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A186" s="14" t="s">
         <v>71</v>
       </c>
@@ -29022,8 +29578,11 @@
       <c r="AX186" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="187" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY186" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="187" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A187" s="14" t="s">
         <v>71</v>
       </c>
@@ -29174,8 +29733,11 @@
       <c r="AX187" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="188" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY187" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="188" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A188" s="14" t="s">
         <v>71</v>
       </c>
@@ -29326,8 +29888,11 @@
       <c r="AX188" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="189" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY188" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="189" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A189" s="14" t="s">
         <v>71</v>
       </c>
@@ -29478,8 +30043,11 @@
       <c r="AX189" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="190" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY189" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="190" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A190" s="14" t="s">
         <v>71</v>
       </c>
@@ -29630,8 +30198,11 @@
       <c r="AX190" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="191" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY190" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="191" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A191" s="14" t="s">
         <v>71</v>
       </c>
@@ -29782,8 +30353,11 @@
       <c r="AX191" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="192" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY191" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="192" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A192" s="14" t="s">
         <v>71</v>
       </c>
@@ -29934,8 +30508,11 @@
       <c r="AX192" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="193" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY192" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="193" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A193" s="14" t="s">
         <v>71</v>
       </c>
@@ -30086,8 +30663,11 @@
       <c r="AX193" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="194" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY193" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="194" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A194" s="14" t="s">
         <v>71</v>
       </c>
@@ -30238,8 +30818,11 @@
       <c r="AX194" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="195" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY194" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="195" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A195" s="14" t="s">
         <v>71</v>
       </c>
@@ -30390,8 +30973,11 @@
       <c r="AX195" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="196" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY195" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="196" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A196" s="14" t="s">
         <v>71</v>
       </c>
@@ -30542,8 +31128,11 @@
       <c r="AX196" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="197" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY196" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="197" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A197" s="14" t="s">
         <v>71</v>
       </c>
@@ -30694,8 +31283,11 @@
       <c r="AX197" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="198" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY197" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="198" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A198" s="14" t="s">
         <v>71</v>
       </c>
@@ -30846,8 +31438,11 @@
       <c r="AX198" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="199" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY198" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="199" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A199" s="14" t="s">
         <v>71</v>
       </c>
@@ -30998,8 +31593,11 @@
       <c r="AX199" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="200" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY199" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="200" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A200" s="14" t="s">
         <v>71</v>
       </c>
@@ -31150,8 +31748,11 @@
       <c r="AX200" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="201" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY200" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="201" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A201" s="14" t="s">
         <v>71</v>
       </c>
@@ -31302,8 +31903,11 @@
       <c r="AX201" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="202" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY201" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="202" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A202" s="14" t="s">
         <v>71</v>
       </c>
@@ -31454,8 +32058,11 @@
       <c r="AX202" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="203" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY202" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="203" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A203" s="14" t="s">
         <v>71</v>
       </c>
@@ -31606,8 +32213,11 @@
       <c r="AX203" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="204" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY203" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="204" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A204" s="14" t="s">
         <v>71</v>
       </c>
@@ -31758,8 +32368,11 @@
       <c r="AX204" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="205" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY204" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="205" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A205" s="14" t="s">
         <v>71</v>
       </c>
@@ -31910,8 +32523,11 @@
       <c r="AX205" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="206" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY205" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="206" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A206" s="14" t="s">
         <v>71</v>
       </c>
@@ -32062,8 +32678,11 @@
       <c r="AX206" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="207" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY206" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="207" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A207" s="14" t="s">
         <v>71</v>
       </c>
@@ -32214,8 +32833,11 @@
       <c r="AX207" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="208" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY207" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="208" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A208" s="14" t="s">
         <v>71</v>
       </c>
@@ -32366,8 +32988,11 @@
       <c r="AX208" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="209" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY208" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="209" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A209" s="14" t="s">
         <v>71</v>
       </c>
@@ -32518,8 +33143,11 @@
       <c r="AX209" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="210" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY209" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="210" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A210" s="14" t="s">
         <v>71</v>
       </c>
@@ -32670,8 +33298,11 @@
       <c r="AX210" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="211" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY210" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="211" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A211" s="14" t="s">
         <v>71</v>
       </c>
@@ -32822,8 +33453,11 @@
       <c r="AX211" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="212" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY211" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="212" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A212" s="14" t="s">
         <v>71</v>
       </c>
@@ -32974,8 +33608,11 @@
       <c r="AX212" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="213" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY212" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="213" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A213" s="14" t="s">
         <v>71</v>
       </c>
@@ -33126,8 +33763,11 @@
       <c r="AX213" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="214" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY213" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="214" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A214" s="14" t="s">
         <v>71</v>
       </c>
@@ -33278,8 +33918,11 @@
       <c r="AX214" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="215" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY214" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="215" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A215" s="14" t="s">
         <v>71</v>
       </c>
@@ -33430,8 +34073,11 @@
       <c r="AX215" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="216" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY215" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="216" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A216" s="14" t="s">
         <v>71</v>
       </c>
@@ -33582,8 +34228,11 @@
       <c r="AX216" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="217" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+      <c r="AY216" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="217" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A217" s="14"/>
       <c r="B217" s="15"/>
       <c r="C217" s="15"/>
@@ -33601,7 +34250,7 @@
       <c r="AF217" s="22"/>
       <c r="AL217" s="14"/>
     </row>
-    <row r="218" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="218" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A218" s="14"/>
       <c r="B218" s="15"/>
       <c r="C218" s="15"/>
@@ -33619,7 +34268,7 @@
       <c r="AF218" s="22"/>
       <c r="AL218" s="14"/>
     </row>
-    <row r="219" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="219" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A219" s="14"/>
       <c r="B219" s="15"/>
       <c r="C219" s="15"/>
@@ -33637,7 +34286,7 @@
       <c r="AF219" s="22"/>
       <c r="AL219" s="14"/>
     </row>
-    <row r="220" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="220" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A220" s="14"/>
       <c r="B220" s="15"/>
       <c r="C220" s="15"/>
@@ -33655,7 +34304,7 @@
       <c r="AF220" s="22"/>
       <c r="AL220" s="14"/>
     </row>
-    <row r="221" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="221" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A221" s="14"/>
       <c r="B221" s="15"/>
       <c r="C221" s="15"/>
@@ -33673,7 +34322,7 @@
       <c r="AF221" s="22"/>
       <c r="AL221" s="14"/>
     </row>
-    <row r="222" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="222" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A222" s="14"/>
       <c r="B222" s="15"/>
       <c r="C222" s="15"/>
@@ -33691,7 +34340,7 @@
       <c r="AF222" s="22"/>
       <c r="AL222" s="14"/>
     </row>
-    <row r="223" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="223" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A223" s="14"/>
       <c r="B223" s="15"/>
       <c r="C223" s="15"/>
@@ -33709,7 +34358,7 @@
       <c r="AF223" s="22"/>
       <c r="AL223" s="14"/>
     </row>
-    <row r="224" spans="1:50" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
+    <row r="224" spans="1:51" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.6">
       <c r="A224" s="14"/>
       <c r="B224" s="15"/>
       <c r="C224" s="15"/>

</xml_diff>